<commit_message>
set TN 05 for site level as well
</commit_message>
<xml_diff>
--- a/final carbon data/env_site_final.xlsx
+++ b/final carbon data/env_site_final.xlsx
@@ -5888,7 +5888,9 @@
       <c r="P85" t="n">
         <v>8</v>
       </c>
-      <c r="Q85"/>
+      <c r="Q85" t="n">
+        <v>3</v>
+      </c>
       <c r="R85" t="n">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
nevermind, temporarily set TN 05 through code
</commit_message>
<xml_diff>
--- a/final carbon data/env_site_final.xlsx
+++ b/final carbon data/env_site_final.xlsx
@@ -5889,7 +5889,7 @@
         <v>8</v>
       </c>
       <c r="Q85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R85" t="n">
         <v>91</v>
@@ -5947,9 +5947,7 @@
       <c r="P86" t="n">
         <v>14</v>
       </c>
-      <c r="Q86" t="n">
-        <v>3</v>
-      </c>
+      <c r="Q86"/>
       <c r="R86" t="n">
         <v>177</v>
       </c>

</xml_diff>

<commit_message>
check c diff between disturbances
</commit_message>
<xml_diff>
--- a/final carbon data/env_site_final.xlsx
+++ b/final carbon data/env_site_final.xlsx
@@ -3293,7 +3293,7 @@
         <v>6</v>
       </c>
       <c r="Q41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R41" t="n">
         <v>96</v>
@@ -3352,7 +3352,7 @@
         <v>6</v>
       </c>
       <c r="Q42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R42" t="n">
         <v>89</v>
@@ -3765,7 +3765,7 @@
         <v>6</v>
       </c>
       <c r="Q49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R49" t="n">
         <v>82</v>
@@ -3824,7 +3824,7 @@
         <v>8</v>
       </c>
       <c r="Q50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R50" t="n">
         <v>78</v>
@@ -4001,7 +4001,7 @@
         <v>6</v>
       </c>
       <c r="Q53" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R53" t="n">
         <v>104</v>
@@ -4532,7 +4532,7 @@
         <v>6</v>
       </c>
       <c r="Q62" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R62" t="n">
         <v>111</v>
@@ -5299,7 +5299,7 @@
         <v>1</v>
       </c>
       <c r="Q75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R75" t="n">
         <v>92</v>
@@ -5417,7 +5417,7 @@
         <v>8</v>
       </c>
       <c r="Q77" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R77" t="n">
         <v>83</v>
@@ -5594,7 +5594,7 @@
         <v>1</v>
       </c>
       <c r="Q80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R80" t="n">
         <v>65</v>
@@ -5653,7 +5653,7 @@
         <v>1</v>
       </c>
       <c r="Q81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R81" t="n">
         <v>100</v>
@@ -5712,7 +5712,7 @@
         <v>8</v>
       </c>
       <c r="Q82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R82" t="n">
         <v>88</v>

</xml_diff>

<commit_message>
change aspect to abs(180 - ASP)
</commit_message>
<xml_diff>
--- a/final carbon data/env_site_final.xlsx
+++ b/final carbon data/env_site_final.xlsx
@@ -974,7 +974,7 @@
         <v>3115</v>
       </c>
       <c r="K2" t="n">
-        <v>281.30994</v>
+        <v>78.69006</v>
       </c>
       <c r="L2" t="n">
         <v>88</v>
@@ -1151,7 +1151,7 @@
         <v>3271</v>
       </c>
       <c r="K5" t="n">
-        <v>337.61987</v>
+        <v>22.38013</v>
       </c>
       <c r="L5" t="n">
         <v>181</v>
@@ -1210,7 +1210,7 @@
         <v>4759</v>
       </c>
       <c r="K6" t="n">
-        <v>236.7683</v>
+        <v>123.2317</v>
       </c>
       <c r="L6" t="n">
         <v>15</v>
@@ -1328,7 +1328,7 @@
         <v>3129</v>
       </c>
       <c r="K8" t="n">
-        <v>208.61046</v>
+        <v>151.38954</v>
       </c>
       <c r="L8" t="n">
         <v>93</v>
@@ -1446,7 +1446,7 @@
         <v>4641</v>
       </c>
       <c r="K10" t="n">
-        <v>237.20047</v>
+        <v>122.79953</v>
       </c>
       <c r="L10" t="n">
         <v>8</v>
@@ -1623,7 +1623,7 @@
         <v>4509</v>
       </c>
       <c r="K13" t="n">
-        <v>198.43495</v>
+        <v>161.56505</v>
       </c>
       <c r="L13" t="n">
         <v>108</v>
@@ -1682,7 +1682,7 @@
         <v>2775</v>
       </c>
       <c r="K14" t="n">
-        <v>322.59464</v>
+        <v>37.40536</v>
       </c>
       <c r="L14" t="n">
         <v>55</v>
@@ -2036,7 +2036,7 @@
         <v>4120</v>
       </c>
       <c r="K20" t="n">
-        <v>206.56505</v>
+        <v>153.43495</v>
       </c>
       <c r="L20" t="n">
         <v>152</v>
@@ -2095,7 +2095,7 @@
         <v>2776</v>
       </c>
       <c r="K21" t="n">
-        <v>344.0546</v>
+        <v>15.9454</v>
       </c>
       <c r="L21" t="n">
         <v>150</v>
@@ -2213,7 +2213,7 @@
         <v>4602</v>
       </c>
       <c r="K23" t="n">
-        <v>220.03026</v>
+        <v>139.96974</v>
       </c>
       <c r="L23" t="n">
         <v>62</v>
@@ -2272,7 +2272,7 @@
         <v>2468</v>
       </c>
       <c r="K24" t="n">
-        <v>324.86581</v>
+        <v>35.13419</v>
       </c>
       <c r="L24" t="n">
         <v>20</v>
@@ -2331,7 +2331,7 @@
         <v>2624</v>
       </c>
       <c r="K25" t="n">
-        <v>203.19859</v>
+        <v>156.80141</v>
       </c>
       <c r="L25" t="n">
         <v>33</v>
@@ -2449,7 +2449,7 @@
         <v>3883</v>
       </c>
       <c r="K27" t="n">
-        <v>296.56506</v>
+        <v>63.43494</v>
       </c>
       <c r="L27" t="n">
         <v>26</v>
@@ -2567,7 +2567,7 @@
         <v>2953</v>
       </c>
       <c r="K29" t="n">
-        <v>213.69006</v>
+        <v>146.30994</v>
       </c>
       <c r="L29" t="n">
         <v>29</v>
@@ -2685,7 +2685,7 @@
         <v>4481</v>
       </c>
       <c r="K31" t="n">
-        <v>356.18591</v>
+        <v>3.81409000000002</v>
       </c>
       <c r="L31" t="n">
         <v>84</v>
@@ -2744,7 +2744,7 @@
         <v>3115</v>
       </c>
       <c r="K32" t="n">
-        <v>281.30994</v>
+        <v>78.69006</v>
       </c>
       <c r="L32" t="n">
         <v>88</v>
@@ -2803,7 +2803,7 @@
         <v>3611</v>
       </c>
       <c r="K33" t="n">
-        <v>300.96375</v>
+        <v>59.03625</v>
       </c>
       <c r="L33" t="n">
         <v>234</v>
@@ -2862,7 +2862,7 @@
         <v>5206</v>
       </c>
       <c r="K34" t="n">
-        <v>240.94539</v>
+        <v>119.05461</v>
       </c>
       <c r="L34" t="n">
         <v>122</v>
@@ -2921,7 +2921,7 @@
         <v>2155</v>
       </c>
       <c r="K35" t="n">
-        <v>333.43494</v>
+        <v>26.56506</v>
       </c>
       <c r="L35" t="n">
         <v>16</v>
@@ -2980,7 +2980,7 @@
         <v>4051</v>
       </c>
       <c r="K36" t="n">
-        <v>288.43494</v>
+        <v>71.56506</v>
       </c>
       <c r="L36" t="n">
         <v>106</v>
@@ -3098,7 +3098,7 @@
         <v>3497</v>
       </c>
       <c r="K38" t="n">
-        <v>337.61987</v>
+        <v>22.38013</v>
       </c>
       <c r="L38" t="n">
         <v>77</v>
@@ -3157,7 +3157,7 @@
         <v>2919</v>
       </c>
       <c r="K39" t="n">
-        <v>284.74356</v>
+        <v>75.25644</v>
       </c>
       <c r="L39" t="n">
         <v>186</v>
@@ -3216,7 +3216,7 @@
         <v>3832</v>
       </c>
       <c r="K40" t="n">
-        <v>254.74489</v>
+        <v>105.25511</v>
       </c>
       <c r="L40" t="n">
         <v>68</v>
@@ -3275,7 +3275,7 @@
         <v>4056</v>
       </c>
       <c r="K41" t="n">
-        <v>188.74615</v>
+        <v>171.25385</v>
       </c>
       <c r="L41" t="n">
         <v>41</v>
@@ -3452,7 +3452,7 @@
         <v>4018</v>
       </c>
       <c r="K44" t="n">
-        <v>213.69006</v>
+        <v>146.30994</v>
       </c>
       <c r="L44" t="n">
         <v>86</v>
@@ -3570,7 +3570,7 @@
         <v>3283</v>
       </c>
       <c r="K46" t="n">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="L46" t="n">
         <v>174</v>
@@ -3629,7 +3629,7 @@
         <v>3827</v>
       </c>
       <c r="K47" t="n">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="L47" t="n">
         <v>103</v>
@@ -3747,7 +3747,7 @@
         <v>4089</v>
       </c>
       <c r="K49" t="n">
-        <v>244.98311</v>
+        <v>115.01689</v>
       </c>
       <c r="L49" t="n">
         <v>106</v>
@@ -3806,7 +3806,7 @@
         <v>4066</v>
       </c>
       <c r="K50" t="n">
-        <v>243.43495</v>
+        <v>116.56505</v>
       </c>
       <c r="L50" t="n">
         <v>163</v>
@@ -3865,7 +3865,7 @@
         <v>3845</v>
       </c>
       <c r="K51" t="n">
-        <v>201.80141</v>
+        <v>158.19859</v>
       </c>
       <c r="L51" t="n">
         <v>6</v>
@@ -3924,7 +3924,7 @@
         <v>3811</v>
       </c>
       <c r="K52" t="n">
-        <v>288.43494</v>
+        <v>71.56506</v>
       </c>
       <c r="L52" t="n">
         <v>80</v>
@@ -3983,7 +3983,7 @@
         <v>3977</v>
       </c>
       <c r="K53" t="n">
-        <v>230.71059</v>
+        <v>129.28941</v>
       </c>
       <c r="L53" t="n">
         <v>23</v>
@@ -4042,7 +4042,7 @@
         <v>4166</v>
       </c>
       <c r="K54" t="n">
-        <v>247.83365</v>
+        <v>112.16635</v>
       </c>
       <c r="L54" t="n">
         <v>150</v>
@@ -4160,7 +4160,7 @@
         <v>4535</v>
       </c>
       <c r="K56" t="n">
-        <v>255.96376</v>
+        <v>104.03624</v>
       </c>
       <c r="L56" t="n">
         <v>110</v>
@@ -4219,7 +4219,7 @@
         <v>3648</v>
       </c>
       <c r="K57" t="n">
-        <v>225</v>
+        <v>135</v>
       </c>
       <c r="L57" t="n">
         <v>161</v>
@@ -4278,7 +4278,7 @@
         <v>3266</v>
       </c>
       <c r="K58" t="n">
-        <v>212.00539</v>
+        <v>147.99461</v>
       </c>
       <c r="L58" t="n">
         <v>87</v>
@@ -4396,7 +4396,7 @@
         <v>2192</v>
       </c>
       <c r="K60" t="n">
-        <v>344.74487</v>
+        <v>15.25513</v>
       </c>
       <c r="L60" t="n">
         <v>375</v>
@@ -4455,7 +4455,7 @@
         <v>3872</v>
       </c>
       <c r="K61" t="n">
-        <v>201.80141</v>
+        <v>158.19859</v>
       </c>
       <c r="L61" t="n">
         <v>76</v>
@@ -4514,7 +4514,7 @@
         <v>2797</v>
       </c>
       <c r="K62" t="n">
-        <v>317.33731</v>
+        <v>42.66269</v>
       </c>
       <c r="L62" t="n">
         <v>219</v>
@@ -4573,7 +4573,7 @@
         <v>639</v>
       </c>
       <c r="K63" t="n">
-        <v>334.33481</v>
+        <v>25.66519</v>
       </c>
       <c r="L63" t="n">
         <v>44</v>
@@ -4691,7 +4691,7 @@
         <v>4133</v>
       </c>
       <c r="K65" t="n">
-        <v>296.56506</v>
+        <v>63.43494</v>
       </c>
       <c r="L65" t="n">
         <v>43</v>
@@ -4809,7 +4809,7 @@
         <v>2331</v>
       </c>
       <c r="K67" t="n">
-        <v>302.27563</v>
+        <v>57.72437</v>
       </c>
       <c r="L67" t="n">
         <v>242</v>
@@ -4868,7 +4868,7 @@
         <v>3314</v>
       </c>
       <c r="K68" t="n">
-        <v>251.56505</v>
+        <v>108.43495</v>
       </c>
       <c r="L68" t="n">
         <v>215</v>
@@ -5163,7 +5163,7 @@
         <v>3671</v>
       </c>
       <c r="K73" t="n">
-        <v>244.98311</v>
+        <v>115.01689</v>
       </c>
       <c r="L73" t="n">
         <v>206</v>
@@ -5222,7 +5222,7 @@
         <v>3497</v>
       </c>
       <c r="K74" t="n">
-        <v>210.96376</v>
+        <v>149.03624</v>
       </c>
       <c r="L74" t="n">
         <v>63</v>
@@ -5281,7 +5281,7 @@
         <v>3634</v>
       </c>
       <c r="K75" t="n">
-        <v>249.77515</v>
+        <v>110.22485</v>
       </c>
       <c r="L75" t="n">
         <v>81</v>
@@ -5340,7 +5340,7 @@
         <v>3653</v>
       </c>
       <c r="K76" t="n">
-        <v>288.43494</v>
+        <v>71.56506</v>
       </c>
       <c r="L76" t="n">
         <v>21</v>
@@ -5458,7 +5458,7 @@
         <v>4248</v>
       </c>
       <c r="K78" t="n">
-        <v>225</v>
+        <v>135</v>
       </c>
       <c r="L78" t="n">
         <v>34</v>
@@ -5517,7 +5517,7 @@
         <v>3142</v>
       </c>
       <c r="K79" t="n">
-        <v>208.61046</v>
+        <v>151.38954</v>
       </c>
       <c r="L79" t="n">
         <v>22</v>
@@ -5576,7 +5576,7 @@
         <v>2792</v>
       </c>
       <c r="K80" t="n">
-        <v>355.9144</v>
+        <v>4.0856</v>
       </c>
       <c r="L80" t="n">
         <v>219</v>
@@ -5635,7 +5635,7 @@
         <v>3327</v>
       </c>
       <c r="K81" t="n">
-        <v>1.4688</v>
+        <v>1.46879999999999</v>
       </c>
       <c r="L81" t="n">
         <v>44</v>
@@ -5694,7 +5694,7 @@
         <v>4536</v>
       </c>
       <c r="K82" t="n">
-        <v>198.43495</v>
+        <v>161.56505</v>
       </c>
       <c r="L82" t="n">
         <v>113</v>
@@ -5753,7 +5753,7 @@
         <v>4888</v>
       </c>
       <c r="K83" t="n">
-        <v>192.99461</v>
+        <v>167.00539</v>
       </c>
       <c r="L83" t="n">
         <v>117</v>
@@ -5987,7 +5987,7 @@
         <v>3321</v>
       </c>
       <c r="K87" t="n">
-        <v>348.69006</v>
+        <v>11.30994</v>
       </c>
       <c r="L87" t="n">
         <v>173</v>
@@ -6044,7 +6044,7 @@
         <v>3845</v>
       </c>
       <c r="K88" t="n">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="L88" t="n">
         <v>110</v>

</xml_diff>

<commit_message>
create individual moose level rasters, and create markdown to create raster of space predcting to for each park
</commit_message>
<xml_diff>
--- a/final carbon data/env_site_final.xlsx
+++ b/final carbon data/env_site_final.xlsx
@@ -974,7 +974,7 @@
         <v>3115</v>
       </c>
       <c r="K2" t="n">
-        <v>78.69006</v>
+        <v>101.30994</v>
       </c>
       <c r="L2" t="n">
         <v>88</v>
@@ -1033,7 +1033,7 @@
         <v>4113</v>
       </c>
       <c r="K3" t="n">
-        <v>87.87891</v>
+        <v>92.12109</v>
       </c>
       <c r="L3" t="n">
         <v>61</v>
@@ -1092,7 +1092,7 @@
         <v>5162</v>
       </c>
       <c r="K4" t="n">
-        <v>170.83765</v>
+        <v>9.16235</v>
       </c>
       <c r="L4" t="n">
         <v>88</v>
@@ -1151,7 +1151,7 @@
         <v>3271</v>
       </c>
       <c r="K5" t="n">
-        <v>22.38013</v>
+        <v>157.61987</v>
       </c>
       <c r="L5" t="n">
         <v>181</v>
@@ -1210,7 +1210,7 @@
         <v>4759</v>
       </c>
       <c r="K6" t="n">
-        <v>123.2317</v>
+        <v>56.7683</v>
       </c>
       <c r="L6" t="n">
         <v>15</v>
@@ -1269,7 +1269,7 @@
         <v>3000</v>
       </c>
       <c r="K7" t="n">
-        <v>165.96376</v>
+        <v>14.03624</v>
       </c>
       <c r="L7" t="n">
         <v>19</v>
@@ -1328,7 +1328,7 @@
         <v>3129</v>
       </c>
       <c r="K8" t="n">
-        <v>151.38954</v>
+        <v>28.61046</v>
       </c>
       <c r="L8" t="n">
         <v>93</v>
@@ -1387,7 +1387,7 @@
         <v>2896</v>
       </c>
       <c r="K9" t="n">
-        <v>96.34019</v>
+        <v>83.65981</v>
       </c>
       <c r="L9" t="n">
         <v>110</v>
@@ -1446,7 +1446,7 @@
         <v>4641</v>
       </c>
       <c r="K10" t="n">
-        <v>122.79953</v>
+        <v>57.20047</v>
       </c>
       <c r="L10" t="n">
         <v>8</v>
@@ -1505,7 +1505,7 @@
         <v>3825</v>
       </c>
       <c r="K11" t="n">
-        <v>119.74488</v>
+        <v>60.25512</v>
       </c>
       <c r="L11" t="n">
         <v>23</v>
@@ -1564,7 +1564,7 @@
         <v>3599</v>
       </c>
       <c r="K12" t="n">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="L12" t="n">
         <v>94</v>
@@ -1623,7 +1623,7 @@
         <v>4509</v>
       </c>
       <c r="K13" t="n">
-        <v>161.56505</v>
+        <v>18.43495</v>
       </c>
       <c r="L13" t="n">
         <v>108</v>
@@ -1682,7 +1682,7 @@
         <v>2775</v>
       </c>
       <c r="K14" t="n">
-        <v>37.40536</v>
+        <v>142.59464</v>
       </c>
       <c r="L14" t="n">
         <v>55</v>
@@ -1741,7 +1741,7 @@
         <v>3397</v>
       </c>
       <c r="K15" t="n">
-        <v>146.30994</v>
+        <v>33.69006</v>
       </c>
       <c r="L15" t="n">
         <v>6</v>
@@ -1800,7 +1800,7 @@
         <v>4525</v>
       </c>
       <c r="K16" t="n">
-        <v>161.56505</v>
+        <v>18.43495</v>
       </c>
       <c r="L16" t="n">
         <v>80</v>
@@ -1859,7 +1859,7 @@
         <v>4577</v>
       </c>
       <c r="K17" t="n">
-        <v>178.36342</v>
+        <v>1.63658000000001</v>
       </c>
       <c r="L17" t="n">
         <v>105</v>
@@ -1918,7 +1918,7 @@
         <v>2465</v>
       </c>
       <c r="K18" t="n">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="L18" t="n">
         <v>101</v>
@@ -1977,7 +1977,7 @@
         <v>4949</v>
       </c>
       <c r="K19" t="n">
-        <v>161.56505</v>
+        <v>18.43495</v>
       </c>
       <c r="L19" t="n">
         <v>121</v>
@@ -2036,7 +2036,7 @@
         <v>4120</v>
       </c>
       <c r="K20" t="n">
-        <v>153.43495</v>
+        <v>26.56505</v>
       </c>
       <c r="L20" t="n">
         <v>152</v>
@@ -2095,7 +2095,7 @@
         <v>2776</v>
       </c>
       <c r="K21" t="n">
-        <v>15.9454</v>
+        <v>164.0546</v>
       </c>
       <c r="L21" t="n">
         <v>150</v>
@@ -2154,7 +2154,7 @@
         <v>3337</v>
       </c>
       <c r="K22" t="n">
-        <v>18.43495</v>
+        <v>161.56505</v>
       </c>
       <c r="L22" t="n">
         <v>6</v>
@@ -2213,7 +2213,7 @@
         <v>4602</v>
       </c>
       <c r="K23" t="n">
-        <v>139.96974</v>
+        <v>40.03026</v>
       </c>
       <c r="L23" t="n">
         <v>62</v>
@@ -2272,7 +2272,7 @@
         <v>2468</v>
       </c>
       <c r="K24" t="n">
-        <v>35.13419</v>
+        <v>144.86581</v>
       </c>
       <c r="L24" t="n">
         <v>20</v>
@@ -2331,7 +2331,7 @@
         <v>2624</v>
       </c>
       <c r="K25" t="n">
-        <v>156.80141</v>
+        <v>23.19859</v>
       </c>
       <c r="L25" t="n">
         <v>33</v>
@@ -2390,7 +2390,7 @@
         <v>4490</v>
       </c>
       <c r="K26" t="n">
-        <v>108.43495</v>
+        <v>71.56505</v>
       </c>
       <c r="L26" t="n">
         <v>126</v>
@@ -2449,7 +2449,7 @@
         <v>3883</v>
       </c>
       <c r="K27" t="n">
-        <v>63.43494</v>
+        <v>116.56506</v>
       </c>
       <c r="L27" t="n">
         <v>26</v>
@@ -2508,7 +2508,7 @@
         <v>3340</v>
       </c>
       <c r="K28" t="n">
-        <v>157.9321</v>
+        <v>22.0679</v>
       </c>
       <c r="L28" t="n">
         <v>103</v>
@@ -2567,7 +2567,7 @@
         <v>2953</v>
       </c>
       <c r="K29" t="n">
-        <v>146.30994</v>
+        <v>33.69006</v>
       </c>
       <c r="L29" t="n">
         <v>29</v>
@@ -2626,7 +2626,7 @@
         <v>4183</v>
       </c>
       <c r="K30" t="n">
-        <v>153.43495</v>
+        <v>26.56505</v>
       </c>
       <c r="L30" t="n">
         <v>16</v>
@@ -2685,7 +2685,7 @@
         <v>4481</v>
       </c>
       <c r="K31" t="n">
-        <v>3.81409000000002</v>
+        <v>176.18591</v>
       </c>
       <c r="L31" t="n">
         <v>84</v>
@@ -2744,7 +2744,7 @@
         <v>3115</v>
       </c>
       <c r="K32" t="n">
-        <v>78.69006</v>
+        <v>101.30994</v>
       </c>
       <c r="L32" t="n">
         <v>88</v>
@@ -2803,7 +2803,7 @@
         <v>3611</v>
       </c>
       <c r="K33" t="n">
-        <v>59.03625</v>
+        <v>120.96375</v>
       </c>
       <c r="L33" t="n">
         <v>234</v>
@@ -2862,7 +2862,7 @@
         <v>5206</v>
       </c>
       <c r="K34" t="n">
-        <v>119.05461</v>
+        <v>60.94539</v>
       </c>
       <c r="L34" t="n">
         <v>122</v>
@@ -2880,7 +2880,7 @@
         <v>8</v>
       </c>
       <c r="Q34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R34" t="n">
         <v>86</v>
@@ -2921,7 +2921,7 @@
         <v>2155</v>
       </c>
       <c r="K35" t="n">
-        <v>26.56506</v>
+        <v>153.43494</v>
       </c>
       <c r="L35" t="n">
         <v>16</v>
@@ -2939,7 +2939,7 @@
         <v>1</v>
       </c>
       <c r="Q35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R35" t="n">
         <v>105</v>
@@ -2980,7 +2980,7 @@
         <v>4051</v>
       </c>
       <c r="K36" t="n">
-        <v>71.56506</v>
+        <v>108.43494</v>
       </c>
       <c r="L36" t="n">
         <v>106</v>
@@ -2998,7 +2998,7 @@
         <v>8</v>
       </c>
       <c r="Q36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R36" t="n">
         <v>79</v>
@@ -3039,7 +3039,7 @@
         <v>6356</v>
       </c>
       <c r="K37" t="n">
-        <v>171.25385</v>
+        <v>8.74615</v>
       </c>
       <c r="L37" t="n">
         <v>218</v>
@@ -3057,7 +3057,7 @@
         <v>8</v>
       </c>
       <c r="Q37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R37" t="n">
         <v>110</v>
@@ -3098,7 +3098,7 @@
         <v>3497</v>
       </c>
       <c r="K38" t="n">
-        <v>22.38013</v>
+        <v>157.61987</v>
       </c>
       <c r="L38" t="n">
         <v>77</v>
@@ -3116,7 +3116,7 @@
         <v>6</v>
       </c>
       <c r="Q38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R38" t="n">
         <v>84</v>
@@ -3157,7 +3157,7 @@
         <v>2919</v>
       </c>
       <c r="K39" t="n">
-        <v>75.25644</v>
+        <v>104.74356</v>
       </c>
       <c r="L39" t="n">
         <v>186</v>
@@ -3175,7 +3175,7 @@
         <v>1</v>
       </c>
       <c r="Q39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R39" t="n">
         <v>75</v>
@@ -3216,7 +3216,7 @@
         <v>3832</v>
       </c>
       <c r="K40" t="n">
-        <v>105.25511</v>
+        <v>74.74489</v>
       </c>
       <c r="L40" t="n">
         <v>68</v>
@@ -3234,7 +3234,7 @@
         <v>6</v>
       </c>
       <c r="Q40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R40" t="n">
         <v>147</v>
@@ -3275,7 +3275,7 @@
         <v>4056</v>
       </c>
       <c r="K41" t="n">
-        <v>171.25385</v>
+        <v>8.74615</v>
       </c>
       <c r="L41" t="n">
         <v>41</v>
@@ -3293,7 +3293,7 @@
         <v>6</v>
       </c>
       <c r="Q41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R41" t="n">
         <v>96</v>
@@ -3334,7 +3334,7 @@
         <v>4336</v>
       </c>
       <c r="K42" t="n">
-        <v>75.06858</v>
+        <v>104.93142</v>
       </c>
       <c r="L42" t="n">
         <v>106</v>
@@ -3352,7 +3352,7 @@
         <v>6</v>
       </c>
       <c r="Q42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R42" t="n">
         <v>89</v>
@@ -3393,7 +3393,7 @@
         <v>3832</v>
       </c>
       <c r="K43" t="n">
-        <v>53.1301</v>
+        <v>126.8699</v>
       </c>
       <c r="L43" t="n">
         <v>93</v>
@@ -3411,7 +3411,7 @@
         <v>6</v>
       </c>
       <c r="Q43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R43" t="n">
         <v>71</v>
@@ -3452,7 +3452,7 @@
         <v>4018</v>
       </c>
       <c r="K44" t="n">
-        <v>146.30994</v>
+        <v>33.69006</v>
       </c>
       <c r="L44" t="n">
         <v>86</v>
@@ -3470,7 +3470,7 @@
         <v>1</v>
       </c>
       <c r="Q44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R44" t="n">
         <v>99</v>
@@ -3511,7 +3511,7 @@
         <v>5087</v>
       </c>
       <c r="K45" t="n">
-        <v>167.82854</v>
+        <v>12.17146</v>
       </c>
       <c r="L45" t="n">
         <v>155</v>
@@ -3529,7 +3529,7 @@
         <v>6</v>
       </c>
       <c r="Q45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R45" t="n">
         <v>77</v>
@@ -3570,7 +3570,7 @@
         <v>3283</v>
       </c>
       <c r="K46" t="n">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="L46" t="n">
         <v>174</v>
@@ -3588,7 +3588,7 @@
         <v>1</v>
       </c>
       <c r="Q46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R46" t="n">
         <v>107.61799</v>
@@ -3629,7 +3629,7 @@
         <v>3827</v>
       </c>
       <c r="K47" t="n">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="L47" t="n">
         <v>103</v>
@@ -3647,7 +3647,7 @@
         <v>8</v>
       </c>
       <c r="Q47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R47" t="n">
         <v>71</v>
@@ -3688,7 +3688,7 @@
         <v>4280</v>
       </c>
       <c r="K48" t="n">
-        <v>172.34935</v>
+        <v>7.65065000000001</v>
       </c>
       <c r="L48" t="n">
         <v>57</v>
@@ -3706,7 +3706,7 @@
         <v>8</v>
       </c>
       <c r="Q48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R48" t="n">
         <v>96</v>
@@ -3747,7 +3747,7 @@
         <v>4089</v>
       </c>
       <c r="K49" t="n">
-        <v>115.01689</v>
+        <v>64.98311</v>
       </c>
       <c r="L49" t="n">
         <v>106</v>
@@ -3765,7 +3765,7 @@
         <v>6</v>
       </c>
       <c r="Q49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R49" t="n">
         <v>82</v>
@@ -3806,7 +3806,7 @@
         <v>4066</v>
       </c>
       <c r="K50" t="n">
-        <v>116.56505</v>
+        <v>63.43495</v>
       </c>
       <c r="L50" t="n">
         <v>163</v>
@@ -3824,7 +3824,7 @@
         <v>8</v>
       </c>
       <c r="Q50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R50" t="n">
         <v>78</v>
@@ -3865,7 +3865,7 @@
         <v>3845</v>
       </c>
       <c r="K51" t="n">
-        <v>158.19859</v>
+        <v>21.80141</v>
       </c>
       <c r="L51" t="n">
         <v>6</v>
@@ -3883,7 +3883,7 @@
         <v>1</v>
       </c>
       <c r="Q51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R51" t="n">
         <v>105</v>
@@ -3924,7 +3924,7 @@
         <v>3811</v>
       </c>
       <c r="K52" t="n">
-        <v>71.56506</v>
+        <v>108.43494</v>
       </c>
       <c r="L52" t="n">
         <v>80</v>
@@ -3942,7 +3942,7 @@
         <v>6</v>
       </c>
       <c r="Q52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R52" t="n">
         <v>81</v>
@@ -3983,7 +3983,7 @@
         <v>3977</v>
       </c>
       <c r="K53" t="n">
-        <v>129.28941</v>
+        <v>50.71059</v>
       </c>
       <c r="L53" t="n">
         <v>23</v>
@@ -4001,7 +4001,7 @@
         <v>6</v>
       </c>
       <c r="Q53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R53" t="n">
         <v>104</v>
@@ -4042,7 +4042,7 @@
         <v>4166</v>
       </c>
       <c r="K54" t="n">
-        <v>112.16635</v>
+        <v>67.83365</v>
       </c>
       <c r="L54" t="n">
         <v>150</v>
@@ -4060,7 +4060,7 @@
         <v>6</v>
       </c>
       <c r="Q54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R54" t="n">
         <v>94</v>
@@ -4101,7 +4101,7 @@
         <v>3324</v>
       </c>
       <c r="K55" t="n">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="L55" t="n">
         <v>71</v>
@@ -4119,7 +4119,7 @@
         <v>1</v>
       </c>
       <c r="Q55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R55" t="n">
         <v>86</v>
@@ -4160,7 +4160,7 @@
         <v>4535</v>
       </c>
       <c r="K56" t="n">
-        <v>104.03624</v>
+        <v>75.96376</v>
       </c>
       <c r="L56" t="n">
         <v>110</v>
@@ -4178,7 +4178,7 @@
         <v>8</v>
       </c>
       <c r="Q56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R56" t="n">
         <v>83</v>
@@ -4219,7 +4219,7 @@
         <v>3648</v>
       </c>
       <c r="K57" t="n">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="L57" t="n">
         <v>161</v>
@@ -4237,7 +4237,7 @@
         <v>8</v>
       </c>
       <c r="Q57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R57" t="n">
         <v>83</v>
@@ -4278,7 +4278,7 @@
         <v>3266</v>
       </c>
       <c r="K58" t="n">
-        <v>147.99461</v>
+        <v>32.00539</v>
       </c>
       <c r="L58" t="n">
         <v>87</v>
@@ -4296,7 +4296,7 @@
         <v>6</v>
       </c>
       <c r="Q58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R58" t="n">
         <v>81</v>
@@ -4337,7 +4337,7 @@
         <v>3699</v>
       </c>
       <c r="K59" t="n">
-        <v>106.26021</v>
+        <v>73.73979</v>
       </c>
       <c r="L59" t="n">
         <v>444</v>
@@ -4355,7 +4355,7 @@
         <v>8</v>
       </c>
       <c r="Q59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R59" t="n">
         <v>81</v>
@@ -4396,7 +4396,7 @@
         <v>2192</v>
       </c>
       <c r="K60" t="n">
-        <v>15.25513</v>
+        <v>164.74487</v>
       </c>
       <c r="L60" t="n">
         <v>375</v>
@@ -4414,7 +4414,7 @@
         <v>1</v>
       </c>
       <c r="Q60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R60" t="n">
         <v>100.85822</v>
@@ -4455,7 +4455,7 @@
         <v>3872</v>
       </c>
       <c r="K61" t="n">
-        <v>158.19859</v>
+        <v>21.80141</v>
       </c>
       <c r="L61" t="n">
         <v>76</v>
@@ -4473,7 +4473,7 @@
         <v>1</v>
       </c>
       <c r="Q61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R61" t="n">
         <v>54</v>
@@ -4514,7 +4514,7 @@
         <v>2797</v>
       </c>
       <c r="K62" t="n">
-        <v>42.66269</v>
+        <v>137.33731</v>
       </c>
       <c r="L62" t="n">
         <v>219</v>
@@ -4532,7 +4532,7 @@
         <v>6</v>
       </c>
       <c r="Q62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R62" t="n">
         <v>111</v>
@@ -4573,7 +4573,7 @@
         <v>639</v>
       </c>
       <c r="K63" t="n">
-        <v>25.66519</v>
+        <v>154.33481</v>
       </c>
       <c r="L63" t="n">
         <v>44</v>
@@ -4591,7 +4591,7 @@
         <v>1</v>
       </c>
       <c r="Q63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R63" t="n">
         <v>84</v>
@@ -4650,7 +4650,7 @@
         <v>1</v>
       </c>
       <c r="Q64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R64" t="n">
         <v>109</v>
@@ -4691,7 +4691,7 @@
         <v>4133</v>
       </c>
       <c r="K65" t="n">
-        <v>63.43494</v>
+        <v>116.56506</v>
       </c>
       <c r="L65" t="n">
         <v>43</v>
@@ -4709,7 +4709,7 @@
         <v>8</v>
       </c>
       <c r="Q65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R65" t="n">
         <v>71</v>
@@ -4750,7 +4750,7 @@
         <v>3006</v>
       </c>
       <c r="K66" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="L66" t="n">
         <v>30</v>
@@ -4768,7 +4768,7 @@
         <v>6</v>
       </c>
       <c r="Q66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R66" t="n">
         <v>113</v>
@@ -4809,7 +4809,7 @@
         <v>2331</v>
       </c>
       <c r="K67" t="n">
-        <v>57.72437</v>
+        <v>122.27563</v>
       </c>
       <c r="L67" t="n">
         <v>242</v>
@@ -4827,7 +4827,7 @@
         <v>1</v>
       </c>
       <c r="Q67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R67" t="n">
         <v>85</v>
@@ -4868,7 +4868,7 @@
         <v>3314</v>
       </c>
       <c r="K68" t="n">
-        <v>108.43495</v>
+        <v>71.56505</v>
       </c>
       <c r="L68" t="n">
         <v>215</v>
@@ -4886,7 +4886,7 @@
         <v>1</v>
       </c>
       <c r="Q68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R68" t="n">
         <v>112</v>
@@ -4927,7 +4927,7 @@
         <v>3779</v>
       </c>
       <c r="K69" t="n">
-        <v>108.43495</v>
+        <v>71.56505</v>
       </c>
       <c r="L69" t="n">
         <v>239</v>
@@ -4945,7 +4945,7 @@
         <v>1</v>
       </c>
       <c r="Q69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R69" t="n">
         <v>94</v>
@@ -4986,7 +4986,7 @@
         <v>3465</v>
       </c>
       <c r="K70" t="n">
-        <v>32.47119</v>
+        <v>147.52881</v>
       </c>
       <c r="L70" t="n">
         <v>35</v>
@@ -5004,7 +5004,7 @@
         <v>6</v>
       </c>
       <c r="Q70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R70" t="n">
         <v>83</v>
@@ -5063,7 +5063,7 @@
         <v>8</v>
       </c>
       <c r="Q71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R71" t="n">
         <v>77</v>
@@ -5104,7 +5104,7 @@
         <v>3845</v>
       </c>
       <c r="K72" t="n">
-        <v>26.56505</v>
+        <v>153.43495</v>
       </c>
       <c r="L72" t="n">
         <v>84</v>
@@ -5122,7 +5122,7 @@
         <v>8</v>
       </c>
       <c r="Q72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R72" t="n">
         <v>79</v>
@@ -5163,7 +5163,7 @@
         <v>3671</v>
       </c>
       <c r="K73" t="n">
-        <v>115.01689</v>
+        <v>64.98311</v>
       </c>
       <c r="L73" t="n">
         <v>206</v>
@@ -5181,7 +5181,7 @@
         <v>8</v>
       </c>
       <c r="Q73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R73" t="n">
         <v>84</v>
@@ -5222,7 +5222,7 @@
         <v>3497</v>
       </c>
       <c r="K74" t="n">
-        <v>149.03624</v>
+        <v>30.96376</v>
       </c>
       <c r="L74" t="n">
         <v>63</v>
@@ -5240,7 +5240,7 @@
         <v>6</v>
       </c>
       <c r="Q74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R74" t="n">
         <v>77</v>
@@ -5281,7 +5281,7 @@
         <v>3634</v>
       </c>
       <c r="K75" t="n">
-        <v>110.22485</v>
+        <v>69.77515</v>
       </c>
       <c r="L75" t="n">
         <v>81</v>
@@ -5299,7 +5299,7 @@
         <v>1</v>
       </c>
       <c r="Q75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R75" t="n">
         <v>92</v>
@@ -5340,7 +5340,7 @@
         <v>3653</v>
       </c>
       <c r="K76" t="n">
-        <v>71.56506</v>
+        <v>108.43494</v>
       </c>
       <c r="L76" t="n">
         <v>21</v>
@@ -5358,7 +5358,7 @@
         <v>1</v>
       </c>
       <c r="Q76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R76" t="n">
         <v>101.44521</v>
@@ -5399,7 +5399,7 @@
         <v>4274</v>
       </c>
       <c r="K77" t="n">
-        <v>23.19859</v>
+        <v>156.80141</v>
       </c>
       <c r="L77" t="n">
         <v>171</v>
@@ -5417,7 +5417,7 @@
         <v>8</v>
       </c>
       <c r="Q77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R77" t="n">
         <v>83</v>
@@ -5458,7 +5458,7 @@
         <v>4248</v>
       </c>
       <c r="K78" t="n">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="L78" t="n">
         <v>34</v>
@@ -5476,7 +5476,7 @@
         <v>6</v>
       </c>
       <c r="Q78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R78" t="n">
         <v>99</v>
@@ -5517,7 +5517,7 @@
         <v>3142</v>
       </c>
       <c r="K79" t="n">
-        <v>151.38954</v>
+        <v>28.61046</v>
       </c>
       <c r="L79" t="n">
         <v>22</v>
@@ -5535,7 +5535,7 @@
         <v>1</v>
       </c>
       <c r="Q79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R79" t="n">
         <v>114</v>
@@ -5576,7 +5576,7 @@
         <v>2792</v>
       </c>
       <c r="K80" t="n">
-        <v>4.0856</v>
+        <v>175.9144</v>
       </c>
       <c r="L80" t="n">
         <v>219</v>
@@ -5594,7 +5594,7 @@
         <v>1</v>
       </c>
       <c r="Q80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R80" t="n">
         <v>65</v>
@@ -5635,7 +5635,7 @@
         <v>3327</v>
       </c>
       <c r="K81" t="n">
-        <v>1.46879999999999</v>
+        <v>178.5312</v>
       </c>
       <c r="L81" t="n">
         <v>44</v>
@@ -5694,7 +5694,7 @@
         <v>4536</v>
       </c>
       <c r="K82" t="n">
-        <v>161.56505</v>
+        <v>18.43495</v>
       </c>
       <c r="L82" t="n">
         <v>113</v>
@@ -5712,7 +5712,7 @@
         <v>8</v>
       </c>
       <c r="Q82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R82" t="n">
         <v>88</v>
@@ -5753,7 +5753,7 @@
         <v>4888</v>
       </c>
       <c r="K83" t="n">
-        <v>167.00539</v>
+        <v>12.99461</v>
       </c>
       <c r="L83" t="n">
         <v>117</v>
@@ -5771,7 +5771,7 @@
         <v>8</v>
       </c>
       <c r="Q83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R83" t="n">
         <v>83</v>
@@ -5812,7 +5812,7 @@
         <v>4545</v>
       </c>
       <c r="K84" t="n">
-        <v>150.64224</v>
+        <v>29.35776</v>
       </c>
       <c r="L84" t="n">
         <v>36</v>
@@ -5830,7 +5830,7 @@
         <v>8</v>
       </c>
       <c r="Q84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R84" t="n">
         <v>110</v>
@@ -5871,7 +5871,7 @@
         <v>5335</v>
       </c>
       <c r="K85" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="L85" t="n">
         <v>93</v>
@@ -5987,7 +5987,7 @@
         <v>3321</v>
       </c>
       <c r="K87" t="n">
-        <v>11.30994</v>
+        <v>168.69006</v>
       </c>
       <c r="L87" t="n">
         <v>173</v>
@@ -6044,7 +6044,7 @@
         <v>3845</v>
       </c>
       <c r="K88" t="n">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="L88" t="n">
         <v>110</v>

</xml_diff>